<commit_message>
include two complementary feeding types and food insecure fraction
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="78">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -245,10 +245,10 @@
     <t>Vitamin A supplementation</t>
   </si>
   <si>
-    <t>Complementary feeding</t>
-  </si>
-  <si>
-    <t>IPTp</t>
+    <t>Complementary feeding (education)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (supplementation)</t>
   </si>
   <si>
     <t>Balanced energy supplementation</t>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>pregnant women</t>
+  </si>
+  <si>
+    <t>Food insecure fraction</t>
   </si>
   <si>
     <t>Outcome</t>
@@ -348,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -388,9 +391,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1176,8 +1176,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="37.86"/>
-    <col customWidth="1" min="2" max="2" width="20.71"/>
-    <col customWidth="1" min="3" max="4" width="21.43"/>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
+    <col customWidth="1" min="3" max="3" width="20.57"/>
+    <col customWidth="1" min="4" max="4" width="20.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1202,10 +1203,10 @@
         <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="D2" s="3">
-        <v>100.0</v>
+        <v>7.08</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="12"/>
@@ -1216,13 +1217,13 @@
         <v>57</v>
       </c>
       <c r="B3" s="3">
-        <v>0.97</v>
+        <v>0.621</v>
       </c>
       <c r="C3" s="3">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="D3" s="3">
-        <v>63.47</v>
+        <v>0.35</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="12"/>
@@ -1233,13 +1234,13 @@
         <v>58</v>
       </c>
       <c r="B4" s="3">
-        <v>0.21</v>
+        <v>0.247</v>
       </c>
       <c r="C4" s="3">
         <v>0.85</v>
       </c>
       <c r="D4" s="3">
-        <v>313.75</v>
+        <v>3.91</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="12"/>
@@ -1247,16 +1248,16 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
-        <v>0.61</v>
+        <v>0.0</v>
       </c>
       <c r="C5" s="3">
         <v>0.85</v>
       </c>
       <c r="D5" s="3">
-        <v>325.23</v>
+        <v>230.4</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="12"/>
@@ -1264,16 +1265,16 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3">
-        <v>0.0</v>
+        <v>0.61</v>
       </c>
       <c r="C6" s="3">
         <v>0.85</v>
       </c>
       <c r="D6" s="3">
-        <v>100.0</v>
+        <v>3.91</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="12"/>
@@ -1290,7 +1291,7 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="3">
-        <v>100.0</v>
+        <v>25.0</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="12"/>
@@ -1307,7 +1308,7 @@
         <v>0.85</v>
       </c>
       <c r="D8" s="3">
-        <v>100.0</v>
+        <v>2.15</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="12"/>
@@ -1425,6 +1426,9 @@
     <col customWidth="1" min="1" max="1" width="37.71"/>
     <col customWidth="1" min="2" max="6" width="13.57"/>
     <col customWidth="1" min="7" max="7" width="17.29"/>
+    <col customWidth="1" min="8" max="8" width="9.29"/>
+    <col customWidth="1" min="9" max="9" width="19.57"/>
+    <col customWidth="1" min="10" max="10" width="11.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1449,6 +1453,12 @@
       <c r="G1" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="3">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
@@ -1521,22 +1531,26 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B5" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="13" t="str">
+        <f t="shared" ref="C5:F5" si="1">$J$1</f>
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
       <c r="G5" s="13">
         <v>0.0</v>
@@ -1544,25 +1558,25 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B6" s="13">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" s="13">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="13">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="13">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F6" s="13">
         <v>0.0</v>
       </c>
       <c r="G6" s="13">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -2100,7 +2114,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
@@ -2117,16 +2131,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" s="14">
-        <v>0.35</v>
+        <v>0.31</v>
       </c>
       <c r="D2" s="14">
-        <v>0.35</v>
+        <v>0.31</v>
       </c>
       <c r="E2" s="14">
         <v>0.0</v>
@@ -2137,33 +2151,36 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="15">
-        <v>0.1</v>
+        <v>66</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f>'Interventions target population'!$J$1</f>
+        <v>0.30</v>
+      </c>
+      <c r="D3" s="14" t="str">
+        <f>'Interventions target population'!$J$1</f>
+        <v>0.30</v>
+      </c>
+      <c r="E3" s="14" t="str">
+        <f>'Interventions target population'!$J$1</f>
+        <v>0.30</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" s="14">
-        <v>0.31</v>
+        <v>0.09</v>
       </c>
       <c r="D4" s="14">
-        <v>0.31</v>
+        <v>0.09</v>
       </c>
       <c r="E4" s="14">
         <v>0.0</v>
@@ -2174,55 +2191,18 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="14">
-        <v>0.336</v>
+        <v>1.0</v>
       </c>
       <c r="D5" s="14">
-        <v>0.336</v>
+        <v>1.0</v>
       </c>
       <c r="E5" s="14">
-        <v>0.336</v>
+        <v>1.0</v>
       </c>
       <c r="F5" s="14">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -2243,7 +2223,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2280,10 +2260,10 @@
       <c r="E2" s="3">
         <v>0.0</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <v>0.253</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="15">
         <v>0.253</v>
       </c>
     </row>
@@ -2301,10 +2281,10 @@
       <c r="E3" s="3">
         <v>0.0</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>0.253</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>0.253</v>
       </c>
     </row>
@@ -2324,10 +2304,10 @@
       <c r="E4" s="3">
         <v>0.416</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>0.416</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>0.416</v>
       </c>
     </row>
@@ -2389,7 +2369,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2532,7 +2512,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -2675,19 +2655,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
@@ -2695,7 +2675,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
         <v>3.14</v>
@@ -2710,7 +2690,7 @@
     <row r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3">
         <v>1.6</v>
@@ -2725,7 +2705,7 @@
     <row r="4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3">
         <v>1.6</v>
@@ -2742,7 +2722,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3">
         <v>1.75</v>
@@ -2756,7 +2736,7 @@
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3">
         <v>1.4</v>
@@ -2770,7 +2750,7 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3">
         <v>1.4</v>
@@ -2787,7 +2767,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="3">
         <v>1.52</v>
@@ -2801,7 +2781,7 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3">
         <v>1.2</v>
@@ -2815,7 +2795,7 @@
     </row>
     <row r="10">
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3">
         <v>1.2</v>
@@ -2841,22 +2821,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3">
         <v>0.0543</v>
@@ -2870,7 +2850,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3">
         <v>0.009</v>
@@ -2884,7 +2864,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -2910,16 +2890,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -2950,19 +2930,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
use food secure fraction from demographics
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="83">
   <si>
     <t>indicators</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>pregnant women</t>
-  </si>
-  <si>
-    <t>Food insecure fraction</t>
   </si>
   <si>
     <t>Outcome</t>
@@ -1581,12 +1578,8 @@
       <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -1665,19 +1658,19 @@
         <v>0.0</v>
       </c>
       <c r="C5" s="15" t="str">
-        <f t="shared" ref="C5:F5" si="1">$J$1</f>
+        <f>demographics!$B$5</f>
         <v>0.3</v>
       </c>
       <c r="D5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f>demographics!$B$5</f>
         <v>0.3</v>
       </c>
       <c r="E5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f>demographics!$B$5</f>
         <v>0.3</v>
       </c>
       <c r="F5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f>demographics!$B$5</f>
         <v>0.3</v>
       </c>
       <c r="G5" s="15">
@@ -1870,7 +1863,7 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -1890,7 +1883,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="16">
         <v>0.31</v>
@@ -1907,18 +1900,18 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="16" t="str">
-        <f>'Interventions target population'!$J$1</f>
+        <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
       <c r="D3" s="16" t="str">
-        <f>'Interventions target population'!$J$1</f>
+        <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
       <c r="E3" s="16" t="str">
-        <f>'Interventions target population'!$J$1</f>
+        <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
       <c r="F3" s="16">
@@ -1930,7 +1923,7 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16">
         <v>0.09</v>
@@ -1947,7 +1940,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="16">
         <v>1.0</v>
@@ -1979,7 +1972,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -2125,7 +2118,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -2268,7 +2261,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -2411,19 +2404,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -2431,7 +2424,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2">
         <v>3.14</v>
@@ -2446,7 +2439,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
         <v>1.6</v>
@@ -2461,7 +2454,7 @@
     <row r="4">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2">
         <v>1.6</v>
@@ -2478,7 +2471,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2">
         <v>1.75</v>
@@ -2492,7 +2485,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2">
         <v>1.4</v>
@@ -2506,7 +2499,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2">
         <v>1.4</v>
@@ -2523,7 +2516,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2">
         <v>1.52</v>
@@ -2537,7 +2530,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2">
         <v>1.2</v>
@@ -2551,7 +2544,7 @@
     </row>
     <row r="10">
       <c r="B10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2">
         <v>1.2</v>
@@ -2577,22 +2570,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2">
         <v>0.0543</v>
@@ -2606,7 +2599,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2">
         <v>0.009</v>
@@ -2620,7 +2613,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2">
         <v>0.0</v>
@@ -2646,16 +2639,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2">
@@ -2686,19 +2679,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
fix total mortality and calculation of age-group mortality
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="88">
   <si>
     <t>indicators</t>
   </si>
@@ -97,6 +97,18 @@
     <t>number of births</t>
   </si>
   <si>
+    <t>neonatal</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>under 5</t>
+  </si>
+  <si>
+    <t>Cause</t>
+  </si>
+  <si>
     <t>&lt;1 month</t>
   </si>
   <si>
@@ -110,9 +122,6 @@
   </si>
   <si>
     <t>24-59 months</t>
-  </si>
-  <si>
-    <t>Cause</t>
   </si>
   <si>
     <t>Neonatal diarrhea</t>
@@ -336,7 +345,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -346,6 +355,10 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <name val="Arial"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -377,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -399,6 +412,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -408,16 +424,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -427,10 +443,10 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -628,24 +644,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
         <v>1.0</v>
@@ -664,7 +680,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>1.0</v>
@@ -683,7 +699,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>1.0</v>
@@ -702,7 +718,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>1.0</v>
@@ -721,7 +737,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>1.0</v>
@@ -740,7 +756,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4">
         <v>1.0</v>
@@ -759,7 +775,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4">
         <v>1.0</v>
@@ -778,7 +794,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4">
         <v>1.0</v>
@@ -913,16 +929,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
@@ -953,47 +969,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11">
+        <v>25</v>
+      </c>
+      <c r="B2" s="12">
         <v>0.2</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="12">
         <v>0.2</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>0.3</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="12">
         <v>0.25</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="12">
         <v>0.15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2">
         <v>0.0</v>
@@ -1028,27 +1044,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>1.0</v>
@@ -1068,7 +1084,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>1.26</v>
@@ -1088,7 +1104,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>1.68</v>
@@ -1108,7 +1124,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>2.65</v>
@@ -1140,27 +1156,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1.04</v>
@@ -1191,30 +1207,30 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>44</v>
+      <c r="A1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="13">
+      <c r="A2" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="14">
         <v>2.82</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="14">
         <v>1.94</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>4.98</v>
       </c>
     </row>
@@ -1235,27 +1251,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2">
         <v>1.0</v>
@@ -1314,27 +1330,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2">
         <v>1.0</v>
@@ -1354,7 +1370,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2">
         <v>1.0</v>
@@ -1374,7 +1390,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2">
         <v>1.0</v>
@@ -1394,7 +1410,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2">
         <v>1.0</v>
@@ -1430,41 +1446,41 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="8">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9">
         <v>5.16</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="9">
         <v>5.16</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>1.82</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="15">
         <v>1.82</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="16">
         <v>1.0</v>
       </c>
     </row>
@@ -1501,36 +1517,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="A2" s="9" t="s">
         <v>43</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -1703,23 +1719,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="16">
+        <v>58</v>
+      </c>
+      <c r="B2" s="17">
         <v>0.0</v>
       </c>
       <c r="C2" s="2">
@@ -1729,12 +1745,12 @@
         <v>7.08</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="17"/>
+      <c r="F2" s="18"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2">
         <v>0.621</v>
@@ -1746,12 +1762,12 @@
         <v>0.35</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="17"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2">
         <v>0.247</v>
@@ -1763,12 +1779,12 @@
         <v>3.91</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2">
         <v>0.0</v>
@@ -1780,12 +1796,12 @@
         <v>230.4</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2">
         <v>0.61</v>
@@ -1797,12 +1813,12 @@
         <v>3.91</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2">
         <v>0.0</v>
@@ -1814,12 +1830,12 @@
         <v>25.0</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2">
         <v>0.0</v>
@@ -1831,7 +1847,7 @@
         <v>2.15</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
@@ -1953,32 +1969,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6">
         <v>0.0</v>
@@ -2001,7 +2017,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B3" s="6">
         <v>0.0</v>
@@ -2024,7 +2040,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B4" s="6">
         <v>0.0</v>
@@ -2047,7 +2063,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B5" s="6">
         <v>0.0</v>
@@ -2074,7 +2090,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" s="6">
         <v>1.0</v>
@@ -2097,7 +2113,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B7" s="6">
         <v>0.0</v>
@@ -2120,7 +2136,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6">
         <v>0.0</v>
@@ -2255,98 +2271,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="18">
+        <v>75</v>
+      </c>
+      <c r="C2" s="19">
         <v>0.31</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="19">
         <v>0.31</v>
       </c>
-      <c r="E2" s="18">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="18">
+      <c r="E2" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="18" t="str">
+        <v>76</v>
+      </c>
+      <c r="C3" s="19" t="str">
         <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
-      <c r="D3" s="18" t="str">
+      <c r="D3" s="19" t="str">
         <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
-      <c r="E3" s="18" t="str">
+      <c r="E3" s="19" t="str">
         <f>demographics!$B$5</f>
         <v>0.30</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="18">
+        <v>75</v>
+      </c>
+      <c r="C4" s="19">
         <v>0.09</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="19">
         <v>0.09</v>
       </c>
-      <c r="E4" s="18">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="18">
+      <c r="E4" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="19">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="18">
+        <v>76</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="19">
         <v>0.0</v>
       </c>
     </row>
@@ -2367,33 +2383,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>0.0</v>
@@ -2404,17 +2420,17 @@
       <c r="E2" s="2">
         <v>0.0</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="20">
         <v>0.253</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="20">
         <v>0.253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>0.0</v>
@@ -2425,19 +2441,19 @@
       <c r="E3" s="2">
         <v>0.0</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="20">
         <v>0.253</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="20">
         <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
         <v>0.0</v>
@@ -2448,16 +2464,16 @@
       <c r="E4" s="2">
         <v>0.416</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="21">
         <v>0.416</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="21">
         <v>0.416</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>0.0</v>
@@ -2513,33 +2529,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>0.0</v>
@@ -2560,7 +2576,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>0.0</v>
@@ -2580,10 +2596,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
         <v>0.0</v>
@@ -2603,7 +2619,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>0.0</v>
@@ -2656,33 +2672,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>0.0</v>
@@ -2703,7 +2719,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>0.0</v>
@@ -2723,10 +2739,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
         <v>0.0</v>
@@ -2746,7 +2762,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>0.0</v>
@@ -2799,27 +2815,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2">
         <v>3.14</v>
@@ -2834,7 +2850,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2">
         <v>1.6</v>
@@ -2849,7 +2865,7 @@
     <row r="4">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2">
         <v>1.6</v>
@@ -2863,10 +2879,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2">
         <v>1.75</v>
@@ -2880,7 +2896,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2">
         <v>1.4</v>
@@ -2894,7 +2910,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2">
         <v>1.4</v>
@@ -2908,10 +2924,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2">
         <v>1.52</v>
@@ -2925,7 +2941,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2">
         <v>1.2</v>
@@ -2939,7 +2955,7 @@
     </row>
     <row r="10">
       <c r="B10" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2">
         <v>1.2</v>
@@ -2965,22 +2981,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2">
         <v>0.0543</v>
@@ -2994,7 +3010,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2">
         <v>0.009</v>
@@ -3008,7 +3024,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2">
         <v>0.0</v>
@@ -3034,16 +3050,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -3074,24 +3090,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2">
         <v>1.0</v>
@@ -3108,7 +3124,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2">
         <v>1.0</v>
@@ -3125,7 +3141,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2">
         <v>1.0</v>
@@ -3153,36 +3169,24 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>23.3</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>30.7</v>
       </c>
-      <c r="C2" s="8">
-        <v>30.7</v>
-      </c>
-      <c r="D2" s="8">
-        <v>37.6</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="C2" s="9">
         <v>37.6</v>
       </c>
     </row>
@@ -3201,29 +3205,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="9">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10">
         <v>0.007</v>
       </c>
       <c r="C2" s="2">
@@ -3241,9 +3245,9 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="9">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10">
         <v>0.199</v>
       </c>
       <c r="C3" s="2">
@@ -3261,9 +3265,9 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="9">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10">
         <v>0.059</v>
       </c>
       <c r="C4" s="2">
@@ -3281,9 +3285,9 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="9">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10">
         <v>0.229</v>
       </c>
       <c r="C5" s="2">
@@ -3301,9 +3305,9 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="9">
+        <v>21</v>
+      </c>
+      <c r="B6" s="10">
         <v>0.297</v>
       </c>
       <c r="C6" s="2">
@@ -3321,9 +3325,9 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="9">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10">
         <v>0.006</v>
       </c>
       <c r="C7" s="2">
@@ -3341,9 +3345,9 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="9">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10">
         <v>0.127</v>
       </c>
       <c r="C8" s="2">
@@ -3361,9 +3365,9 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="9">
+        <v>24</v>
+      </c>
+      <c r="B9" s="10">
         <v>0.076</v>
       </c>
       <c r="C9" s="2">
@@ -3381,181 +3385,181 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="9">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="10">
         <v>0.1481</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="10">
         <v>0.1481</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="10">
         <v>0.1481</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>0.1481</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="9">
+        <v>26</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="10">
         <v>0.2883</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="10">
         <v>0.2883</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="10">
         <v>0.2883</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="10">
         <v>0.2883</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="9">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="10">
         <v>0.041</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="10">
         <v>0.041</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="10">
         <v>0.041</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="10">
         <v>0.041</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2">
         <v>0.0</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="10">
         <v>0.05</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="10">
         <v>0.05</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="10">
         <v>0.05</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="10">
         <v>0.05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>0.0</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="10">
         <v>0.006</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="10">
         <v>0.006</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="10">
         <v>0.006</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="10">
         <v>0.006</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
         <v>0.0</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="10">
         <v>0.01</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="10">
         <v>0.01</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="10">
         <v>0.01</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="10">
         <v>0.01</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
         <v>0.0</v>
       </c>
-      <c r="C16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="C16" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="10">
         <v>0.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2">
         <v>0.0</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="10">
         <v>0.1451</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="10">
         <v>0.1451</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="10">
         <v>0.1451</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="10">
         <v>0.1451</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2">
         <v>0.0</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="10">
         <v>0.3115</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="10">
         <v>0.3115</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="10">
         <v>0.3115</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="10">
         <v>0.3115</v>
       </c>
     </row>
@@ -3573,210 +3577,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="10">
+        <v>37</v>
+      </c>
+      <c r="C2" s="11">
         <v>60.67</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="11">
         <v>60.67</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="11">
         <v>47.206</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="11">
         <v>22.921</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="11">
         <v>23.661</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="10">
+        <v>38</v>
+      </c>
+      <c r="C3" s="11">
         <v>21.637</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="11">
         <v>21.637</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="11">
         <v>30.252</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="11">
         <v>27.735</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="11">
         <v>31.069</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10">
+        <v>39</v>
+      </c>
+      <c r="C4" s="11">
         <v>13.337</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>13.337</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="11">
         <v>14.065</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="11">
         <v>30.803</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="11">
         <v>28.443</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="10">
+        <v>40</v>
+      </c>
+      <c r="C5" s="11">
         <v>4.356</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="11">
         <v>4.356</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="11">
         <v>8.477</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="11">
         <v>18.541</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="11">
         <v>16.827</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="10">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11">
         <v>60.66</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>60.66</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="11">
         <v>47.21</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="11">
         <v>22.93</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="11">
         <v>23.66</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="10">
+        <v>38</v>
+      </c>
+      <c r="C7" s="11">
         <v>21.64</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="11">
         <v>21.64</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="11">
         <v>30.25</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="11">
         <v>27.73</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="11">
         <v>31.07</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="10">
+        <v>39</v>
+      </c>
+      <c r="C8" s="11">
         <v>13.34</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>13.34</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <v>14.06</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="11">
         <v>30.8</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <v>28.44</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="10">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11">
         <v>4.36</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <v>4.36</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="11">
         <v>8.48</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="11">
         <v>18.54</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="11">
         <v>16.83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="10">
+        <v>43</v>
+      </c>
+      <c r="C10" s="11">
         <v>87.6</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="11">
         <v>61.0</v>
       </c>
-      <c r="E10" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E10" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="11">
         <v>0.0</v>
       </c>
       <c r="G10" s="4">
@@ -3785,12 +3789,12 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="10">
+        <v>44</v>
+      </c>
+      <c r="C11" s="11">
         <v>3.5</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="11">
         <v>13.9</v>
       </c>
       <c r="E11" s="4">
@@ -3805,18 +3809,18 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="10">
+        <v>45</v>
+      </c>
+      <c r="C12" s="11">
         <v>8.9</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="11">
         <v>24.2</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="11">
         <v>96.4</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="11">
         <v>93.1</v>
       </c>
       <c r="G12" s="4">
@@ -3825,7 +3829,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4">
         <v>0.0</v>
@@ -3833,10 +3837,10 @@
       <c r="D13" s="4">
         <v>1.0</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="11">
         <v>3.6</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="11">
         <v>6.9</v>
       </c>
       <c r="G13" s="4">
@@ -3858,13 +3862,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -3892,33 +3896,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -3938,7 +3942,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
@@ -3958,7 +3962,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -3978,7 +3982,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -3998,10 +4002,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -4021,7 +4025,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -4041,7 +4045,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -4061,7 +4065,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -4081,10 +4085,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -4104,7 +4108,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -4124,7 +4128,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -4144,7 +4148,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
@@ -4164,10 +4168,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
@@ -4187,7 +4191,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
@@ -4207,7 +4211,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
@@ -4227,7 +4231,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
@@ -4247,10 +4251,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -4270,7 +4274,7 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -4290,7 +4294,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -4310,7 +4314,7 @@
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -4342,33 +4346,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -4388,7 +4392,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
@@ -4408,7 +4412,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -4428,7 +4432,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -4448,10 +4452,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -4471,7 +4475,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -4491,7 +4495,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -4511,7 +4515,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -4531,10 +4535,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -4554,7 +4558,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -4574,7 +4578,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
@@ -4594,7 +4598,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
@@ -4614,10 +4618,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
@@ -4637,7 +4641,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
@@ -4657,7 +4661,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
@@ -4677,7 +4681,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
@@ -4697,10 +4701,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -4720,7 +4724,7 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -4740,7 +4744,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -4760,7 +4764,7 @@
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -4795,33 +4799,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>1.0</v>
@@ -4841,7 +4845,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>1.26</v>
@@ -4861,7 +4865,7 @@
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2">
         <v>1.83</v>
@@ -4881,7 +4885,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>10.88</v>
@@ -4901,10 +4905,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>1.0</v>
@@ -4924,7 +4928,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2">
         <v>1.26</v>
@@ -4944,7 +4948,7 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2">
         <v>1.83</v>
@@ -4964,7 +4968,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>10.88</v>
@@ -4984,10 +4988,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>1.0</v>
@@ -5007,7 +5011,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2">
         <v>1.26</v>
@@ -5027,7 +5031,7 @@
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2">
         <v>1.83</v>
@@ -5047,7 +5051,7 @@
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
         <v>10.88</v>
@@ -5067,10 +5071,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>1.0</v>
@@ -5090,7 +5094,7 @@
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2">
         <v>1.26</v>
@@ -5110,7 +5114,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2">
         <v>1.83</v>
@@ -5130,7 +5134,7 @@
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2">
         <v>10.88</v>
@@ -5150,10 +5154,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -5173,7 +5177,7 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -5193,7 +5197,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -5213,7 +5217,7 @@
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -5233,10 +5237,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
@@ -5256,7 +5260,7 @@
     </row>
     <row r="23">
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2">
         <v>1.0</v>
@@ -5276,7 +5280,7 @@
     </row>
     <row r="24">
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2">
         <v>1.0</v>
@@ -5296,7 +5300,7 @@
     </row>
     <row r="25">
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
@@ -5316,10 +5320,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
@@ -5339,7 +5343,7 @@
     </row>
     <row r="27">
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
@@ -5359,7 +5363,7 @@
     </row>
     <row r="28">
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
@@ -5379,7 +5383,7 @@
     </row>
     <row r="29">
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>

</xml_diff>

<commit_message>
fix target pop for comp feeding; accept unusually OR stunting progression
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -946,7 +946,7 @@
         <v>11.2</v>
       </c>
       <c r="B2" s="2">
-        <v>26.9</v>
+        <v>268.7</v>
       </c>
       <c r="C2" s="2">
         <v>67.3</v>
@@ -2046,7 +2046,7 @@
         <v>0.0</v>
       </c>
       <c r="C4" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="6">
         <v>1.0</v>
@@ -2055,7 +2055,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="6">
         <v>0.0</v>
@@ -2068,9 +2068,8 @@
       <c r="B5" s="6">
         <v>0.0</v>
       </c>
-      <c r="C5" s="6" t="str">
-        <f>demographics!$B$5</f>
-        <v>0.3</v>
+      <c r="C5" s="6">
+        <v>0.0</v>
       </c>
       <c r="D5" s="6" t="str">
         <f>demographics!$B$5</f>
@@ -2080,9 +2079,8 @@
         <f>demographics!$B$5</f>
         <v>0.3</v>
       </c>
-      <c r="F5" s="6" t="str">
-        <f>demographics!$B$5</f>
-        <v>0.3</v>
+      <c r="F5" s="6">
+        <v>0.0</v>
       </c>
       <c r="G5" s="6">
         <v>0.0</v>

</xml_diff>

<commit_message>
remove birth time/order worksheets; rename sheet with cost and coverage
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -22,16 +22,12 @@
     <sheet state="visible" name="OR stunting for complements" sheetId="17" r:id="rId19"/>
     <sheet state="visible" name="OR appropriateBF by interv" sheetId="18" r:id="rId20"/>
     <sheet state="visible" name="Appropriate breastfeeding" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions cost and coverage" sheetId="20" r:id="rId22"/>
     <sheet state="visible" name="Interventions target population" sheetId="21" r:id="rId23"/>
     <sheet state="visible" name="Interventions maternal" sheetId="22" r:id="rId24"/>
     <sheet state="visible" name="Interventions affected fraction" sheetId="23" r:id="rId25"/>
     <sheet state="visible" name="Interventions mortality eff" sheetId="24" r:id="rId26"/>
     <sheet state="visible" name="Interventions incidence eff" sheetId="25" r:id="rId27"/>
-    <sheet state="visible" name="RR birth by type" sheetId="26" r:id="rId28"/>
-    <sheet state="visible" name="birth distribution" sheetId="27" r:id="rId29"/>
-    <sheet state="visible" name="time between births" sheetId="28" r:id="rId30"/>
-    <sheet state="visible" name="RR birth by time" sheetId="29" r:id="rId31"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -71,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="78">
   <si>
     <t>indicators</t>
   </si>
@@ -305,36 +301,6 @@
   </si>
   <si>
     <t>Interventions</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>&lt;18 years</t>
-  </si>
-  <si>
-    <t>18-34 years</t>
-  </si>
-  <si>
-    <t>35-49 years</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second or third</t>
-  </si>
-  <si>
-    <t>greater than third</t>
-  </si>
-  <si>
-    <t>&lt;18 months</t>
-  </si>
-  <si>
-    <t>18-23 months</t>
-  </si>
-  <si>
-    <t>&lt;24 months</t>
   </si>
 </sst>
 </file>
@@ -529,22 +495,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing26.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing27.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing28.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing29.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -2804,361 +2754,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.0543</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.1048</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>0.2258</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.0705</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.134</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.5698</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>

</xml_diff>

<commit_message>
update demographics, incidences, mortality, distributions; assume annual incidences (cases per year) instead or monthly
</commit_message>
<xml_diff>
--- a/InputForCode_Bangladesh.xlsx
+++ b/InputForCode_Bangladesh.xlsx
@@ -9,12 +9,12 @@
     <sheet state="visible" name="mortality" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="distributions" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="birth outcome distribution" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="RRStunting" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="RRWasting" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="RRBreastfeeding" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="RR Death by Birth Outcome" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="Incidence of conditions" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="Incidence of conditions" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="RRStunting" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="RRWasting" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="RRBreastfeeding" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="RR Death by Birth Outcome" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="13" r:id="rId15"/>
     <sheet state="visible" name="OR stunting by condition" sheetId="14" r:id="rId16"/>
     <sheet state="visible" name="OR stunting by birth outcome" sheetId="15" r:id="rId17"/>
@@ -219,6 +219,9 @@
     <t>Term SGA</t>
   </si>
   <si>
+    <t>Condition</t>
+  </si>
+  <si>
     <t>Stunting Status</t>
   </si>
   <si>
@@ -232,9 +235,6 @@
   </si>
   <si>
     <t>Neonatal congenital anomalies</t>
-  </si>
-  <si>
-    <t>Condition</t>
   </si>
   <si>
     <t>Breastfeeding Category</t>
@@ -311,7 +311,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -321,6 +321,10 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
       <name val="Arial"/>
@@ -337,12 +341,24 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor rgb="FFFDE9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor rgb="FFDAEEF3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -356,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -366,40 +382,56 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -409,10 +441,10 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -546,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>1.479E7</v>
+        <v>1.5204E7</v>
       </c>
     </row>
     <row r="3">
@@ -554,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>3030000.0</v>
+        <v>3118117.0</v>
       </c>
     </row>
     <row r="4">
@@ -562,7 +594,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>3583822.0</v>
+        <v>3689944.0</v>
       </c>
     </row>
     <row r="5">
@@ -570,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="6">
@@ -582,6 +614,625 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="24.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D18">
+        <v>1.0</v>
+      </c>
+      <c r="E18">
+        <v>1.0</v>
+      </c>
+      <c r="F18">
+        <v>1.0</v>
+      </c>
+      <c r="G18">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="E19">
+        <v>1.0</v>
+      </c>
+      <c r="F19">
+        <v>1.0</v>
+      </c>
+      <c r="G19">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="E20">
+        <v>1.0</v>
+      </c>
+      <c r="F20">
+        <v>1.0</v>
+      </c>
+      <c r="G20">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10.88</v>
+      </c>
+      <c r="E21">
+        <v>2.1</v>
+      </c>
+      <c r="F21">
+        <v>2.1</v>
+      </c>
+      <c r="G21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D22">
+        <v>1.0</v>
+      </c>
+      <c r="E22">
+        <v>1.0</v>
+      </c>
+      <c r="F22">
+        <v>1.0</v>
+      </c>
+      <c r="G22">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D23">
+        <v>1.66</v>
+      </c>
+      <c r="E23">
+        <v>1.0</v>
+      </c>
+      <c r="F23">
+        <v>1.0</v>
+      </c>
+      <c r="G23">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>1.0</v>
+      </c>
+      <c r="F24">
+        <v>1.0</v>
+      </c>
+      <c r="G24">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D25">
+        <v>14.97</v>
+      </c>
+      <c r="E25">
+        <v>1.92</v>
+      </c>
+      <c r="F25">
+        <v>1.92</v>
+      </c>
+      <c r="G25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D26">
+        <v>1.0</v>
+      </c>
+      <c r="E26">
+        <v>1.0</v>
+      </c>
+      <c r="F26">
+        <v>1.0</v>
+      </c>
+      <c r="G26">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D27">
+        <v>1.0</v>
+      </c>
+      <c r="E27">
+        <v>1.0</v>
+      </c>
+      <c r="F27">
+        <v>1.0</v>
+      </c>
+      <c r="G27">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D28">
+        <v>1.0</v>
+      </c>
+      <c r="E28">
+        <v>1.0</v>
+      </c>
+      <c r="F28">
+        <v>1.0</v>
+      </c>
+      <c r="G28">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D29">
+        <v>1.0</v>
+      </c>
+      <c r="E29">
+        <v>1.0</v>
+      </c>
+      <c r="F29">
+        <v>1.0</v>
+      </c>
+      <c r="G29">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -596,8 +1247,8 @@
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>53</v>
+      <c r="B1" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -610,152 +1261,152 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="15">
         <v>1.0</v>
       </c>
       <c r="C2">
         <v>1.0</v>
       </c>
-      <c r="D2" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="15">
         <v>1.0</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="15">
         <v>1.0</v>
       </c>
       <c r="C3">
         <v>2.07</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="15">
         <v>8.02</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="15">
         <v>11.54</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="15">
         <v>1.0</v>
       </c>
       <c r="C4">
         <v>2.07</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="15">
         <v>8.02</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="15">
         <v>11.54</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="15">
         <v>1.0</v>
       </c>
       <c r="C5">
         <v>2.07</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="15">
         <v>8.02</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="15">
         <v>11.54</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="15">
         <v>1.0</v>
       </c>
       <c r="C6">
         <v>1.0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="15">
         <v>999.99</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="15">
         <v>999.99</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="15">
         <v>1.0</v>
       </c>
       <c r="C7">
         <v>1.0</v>
       </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="15">
         <v>1.0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="4">
+      <c r="A8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="15">
         <v>1.0</v>
       </c>
       <c r="C8">
         <v>1.0</v>
       </c>
-      <c r="D8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="15">
         <v>1.0</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="15">
         <v>1.0</v>
       </c>
       <c r="C9">
         <v>1.0</v>
       </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="15">
         <v>1.0</v>
       </c>
       <c r="F9" s="2"/>
@@ -870,7 +1521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -903,78 +1554,6 @@
       </c>
       <c r="D2" s="2">
         <v>67.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="C2" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="E2" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="F2" s="12">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1685,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -1157,30 +1736,30 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="14">
+      <c r="A2" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="17">
         <v>2.82</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="17">
         <v>1.94</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="17">
         <v>4.98</v>
       </c>
     </row>
@@ -1418,19 +1997,19 @@
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="18">
         <v>5.16</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="18">
         <v>5.16</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="18">
         <v>1.82</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="19">
         <v>1.82</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="20">
         <v>1.0</v>
       </c>
     </row>
@@ -1483,19 +2062,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="19" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1542,7 +2121,7 @@
         <v>2017.0</v>
       </c>
       <c r="B2" s="7">
-        <v>3010000.0</v>
+        <v>3095470.0</v>
       </c>
     </row>
     <row r="3">
@@ -1550,7 +2129,7 @@
         <v>2018.0</v>
       </c>
       <c r="B3" s="7">
-        <v>2980000.0</v>
+        <v>3071259.0</v>
       </c>
     </row>
     <row r="4">
@@ -1558,7 +2137,7 @@
         <v>2019.0</v>
       </c>
       <c r="B4" s="7">
-        <v>2960000.0</v>
+        <v>3045241.0</v>
       </c>
     </row>
     <row r="5">
@@ -1566,7 +2145,7 @@
         <v>2020.0</v>
       </c>
       <c r="B5" s="7">
-        <v>2930000.0</v>
+        <v>3017266.0</v>
       </c>
     </row>
     <row r="6">
@@ -1574,7 +2153,7 @@
         <v>2021.0</v>
       </c>
       <c r="B6" s="7">
-        <v>2900000.0</v>
+        <v>2990677.0</v>
       </c>
     </row>
     <row r="7">
@@ -1582,7 +2161,7 @@
         <v>2022.0</v>
       </c>
       <c r="B7" s="7">
-        <v>2870000.0</v>
+        <v>2962144.0</v>
       </c>
     </row>
     <row r="8">
@@ -1590,7 +2169,7 @@
         <v>2023.0</v>
       </c>
       <c r="B8" s="7">
-        <v>2840000.0</v>
+        <v>2931643.0</v>
       </c>
     </row>
     <row r="9">
@@ -1598,7 +2177,7 @@
         <v>2024.0</v>
       </c>
       <c r="B9" s="7">
-        <v>2810000.0</v>
+        <v>2899255.0</v>
       </c>
     </row>
     <row r="10">
@@ -1606,7 +2185,7 @@
         <v>2025.0</v>
       </c>
       <c r="B10" s="7">
-        <v>2780000.0</v>
+        <v>2865008.0</v>
       </c>
     </row>
     <row r="11">
@@ -1614,7 +2193,7 @@
         <v>2026.0</v>
       </c>
       <c r="B11" s="7">
-        <v>2740000.0</v>
+        <v>2836142.0</v>
       </c>
     </row>
     <row r="12">
@@ -1622,7 +2201,7 @@
         <v>2027.0</v>
       </c>
       <c r="B12" s="7">
-        <v>2710000.0</v>
+        <v>2805541.0</v>
       </c>
     </row>
     <row r="13">
@@ -1630,7 +2209,7 @@
         <v>2028.0</v>
       </c>
       <c r="B13" s="7">
-        <v>2670000.0</v>
+        <v>2773236.0</v>
       </c>
     </row>
     <row r="14">
@@ -1638,7 +2217,7 @@
         <v>2029.0</v>
       </c>
       <c r="B14" s="7">
-        <v>2640000.0</v>
+        <v>2739273.0</v>
       </c>
     </row>
     <row r="15">
@@ -1646,7 +2225,7 @@
         <v>2030.0</v>
       </c>
       <c r="B15" s="7">
-        <v>2600000.0</v>
+        <v>2703670.0</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +2264,7 @@
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="21">
         <v>0.0</v>
       </c>
       <c r="C2" s="2">
@@ -1695,7 +2274,7 @@
         <v>7.08</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="18"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3">
@@ -1712,7 +2291,7 @@
         <v>0.35</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="18"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4">
@@ -1729,7 +2308,7 @@
         <v>3.91</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5">
@@ -1746,7 +2325,7 @@
         <v>230.4</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6">
@@ -1763,7 +2342,7 @@
         <v>3.91</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
@@ -1780,11 +2359,11 @@
         <v>25.0</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="18"/>
+      <c r="F7" s="22"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="2">
@@ -1797,7 +2376,7 @@
         <v>2.15</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="18"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
@@ -2023,11 +2602,11 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="F5" s="6">
         <v>0.0</v>
@@ -2083,7 +2662,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="6">
@@ -2234,7 +2813,7 @@
         <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
@@ -2244,16 +2823,16 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="23">
         <v>0.31</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="23">
         <v>0.31</v>
       </c>
-      <c r="E2" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="19">
+      <c r="E2" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="23">
         <v>0.0</v>
       </c>
     </row>
@@ -2261,19 +2840,19 @@
       <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="19" t="str">
+      <c r="C3" s="23" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
-      </c>
-      <c r="D3" s="19" t="str">
+        <v>0.31</v>
+      </c>
+      <c r="D3" s="23" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
-      </c>
-      <c r="E3" s="19" t="str">
+        <v>0.31</v>
+      </c>
+      <c r="E3" s="23" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
-      </c>
-      <c r="F3" s="19">
+        <v>0.31</v>
+      </c>
+      <c r="F3" s="23">
         <v>0.0</v>
       </c>
     </row>
@@ -2284,16 +2863,16 @@
       <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="23">
         <v>0.09</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="23">
         <v>0.09</v>
       </c>
-      <c r="E4" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="E4" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="23">
         <v>0.0</v>
       </c>
     </row>
@@ -2301,16 +2880,16 @@
       <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="19">
+      <c r="C5" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="23">
         <v>0.0</v>
       </c>
     </row>
@@ -2368,10 +2947,10 @@
       <c r="E2" s="2">
         <v>0.0</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="24">
         <v>0.253</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="24">
         <v>0.253</v>
       </c>
     </row>
@@ -2389,10 +2968,10 @@
       <c r="E3" s="2">
         <v>0.0</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="24">
         <v>0.253</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="24">
         <v>0.253</v>
       </c>
     </row>
@@ -2412,10 +2991,10 @@
       <c r="E4" s="2">
         <v>0.416</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="25">
         <v>0.416</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="25">
         <v>0.416</v>
       </c>
     </row>
@@ -2774,13 +3353,13 @@
     </row>
     <row r="2">
       <c r="A2" s="9">
-        <v>23.3</v>
+        <v>25.4</v>
       </c>
       <c r="B2" s="9">
-        <v>30.7</v>
+        <v>34.68</v>
       </c>
       <c r="C2" s="9">
-        <v>37.6</v>
+        <v>32.35</v>
       </c>
     </row>
   </sheetData>
@@ -3199,19 +3778,19 @@
         <v>37</v>
       </c>
       <c r="C2" s="11">
-        <v>60.67</v>
+        <v>63.4</v>
       </c>
       <c r="D2" s="11">
-        <v>60.67</v>
+        <v>63.4</v>
       </c>
       <c r="E2" s="11">
-        <v>47.206</v>
+        <v>49.0</v>
       </c>
       <c r="F2" s="11">
-        <v>22.921</v>
+        <v>28.0</v>
       </c>
       <c r="G2" s="11">
-        <v>23.661</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="3">
@@ -3219,19 +3798,19 @@
         <v>38</v>
       </c>
       <c r="C3" s="11">
-        <v>21.637</v>
+        <v>22.6</v>
       </c>
       <c r="D3" s="11">
-        <v>21.637</v>
+        <v>22.6</v>
       </c>
       <c r="E3" s="11">
-        <v>30.252</v>
+        <v>31.4</v>
       </c>
       <c r="F3" s="11">
-        <v>27.735</v>
+        <v>33.9</v>
       </c>
       <c r="G3" s="11">
-        <v>31.069</v>
+        <v>33.2</v>
       </c>
     </row>
     <row r="4">
@@ -3239,19 +3818,19 @@
         <v>39</v>
       </c>
       <c r="C4" s="11">
-        <v>13.337</v>
+        <v>10.2</v>
       </c>
       <c r="D4" s="11">
-        <v>13.337</v>
+        <v>10.2</v>
       </c>
       <c r="E4" s="11">
-        <v>14.065</v>
+        <v>14.7</v>
       </c>
       <c r="F4" s="11">
-        <v>30.803</v>
+        <v>24.7</v>
       </c>
       <c r="G4" s="11">
-        <v>28.443</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="5">
@@ -3259,19 +3838,19 @@
         <v>40</v>
       </c>
       <c r="C5" s="11">
-        <v>4.356</v>
+        <v>3.8</v>
       </c>
       <c r="D5" s="11">
-        <v>4.356</v>
+        <v>3.8</v>
       </c>
       <c r="E5" s="11">
-        <v>8.477</v>
+        <v>4.9</v>
       </c>
       <c r="F5" s="11">
-        <v>18.541</v>
+        <v>13.4</v>
       </c>
       <c r="G5" s="11">
-        <v>16.827</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="6">
@@ -3281,80 +3860,80 @@
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="11">
-        <v>60.66</v>
-      </c>
-      <c r="D6" s="11">
-        <v>60.66</v>
-      </c>
-      <c r="E6" s="11">
-        <v>47.21</v>
-      </c>
-      <c r="F6" s="11">
-        <v>22.93</v>
-      </c>
-      <c r="G6" s="11">
-        <v>23.66</v>
+      <c r="C6" s="12">
+        <v>56.8</v>
+      </c>
+      <c r="D6" s="12">
+        <v>56.8</v>
+      </c>
+      <c r="E6" s="12">
+        <v>58.6</v>
+      </c>
+      <c r="F6" s="12">
+        <v>54.9</v>
+      </c>
+      <c r="G6" s="12">
+        <v>49.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="11">
-        <v>21.64</v>
-      </c>
-      <c r="D7" s="11">
-        <v>21.64</v>
-      </c>
-      <c r="E7" s="11">
-        <v>30.25</v>
-      </c>
-      <c r="F7" s="11">
-        <v>27.73</v>
-      </c>
-      <c r="G7" s="11">
-        <v>31.07</v>
+      <c r="C7" s="12">
+        <v>23.3</v>
+      </c>
+      <c r="D7" s="12">
+        <v>23.3</v>
+      </c>
+      <c r="E7" s="12">
+        <v>23.1</v>
+      </c>
+      <c r="F7" s="12">
+        <v>30.0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>38.4</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="11">
-        <v>13.34</v>
-      </c>
-      <c r="D8" s="11">
-        <v>13.34</v>
-      </c>
-      <c r="E8" s="11">
-        <v>14.06</v>
-      </c>
-      <c r="F8" s="11">
-        <v>30.8</v>
-      </c>
-      <c r="G8" s="11">
-        <v>28.44</v>
+      <c r="C8" s="12">
+        <v>15.0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>15.0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>12.9</v>
+      </c>
+      <c r="F8" s="12">
+        <v>11.0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>10.5</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="11">
-        <v>4.36</v>
-      </c>
-      <c r="D9" s="11">
-        <v>4.36</v>
-      </c>
-      <c r="E9" s="11">
-        <v>8.48</v>
-      </c>
-      <c r="F9" s="11">
-        <v>18.54</v>
-      </c>
-      <c r="G9" s="11">
-        <v>16.83</v>
+      <c r="C9" s="12">
+        <v>4.9</v>
+      </c>
+      <c r="D9" s="12">
+        <v>4.9</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4.1</v>
+      </c>
+      <c r="G9" s="12">
+        <v>2.1</v>
       </c>
     </row>
     <row r="10">
@@ -3364,17 +3943,17 @@
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="11">
-        <v>87.6</v>
-      </c>
-      <c r="D10" s="11">
-        <v>61.0</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0.0</v>
+      <c r="C10" s="13">
+        <v>80.3</v>
+      </c>
+      <c r="D10" s="13">
+        <v>46.2</v>
+      </c>
+      <c r="E10" s="13">
+        <v>3.3</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.7</v>
       </c>
       <c r="G10" s="4">
         <v>0.0</v>
@@ -3384,17 +3963,17 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="D11" s="11">
-        <v>13.9</v>
+      <c r="C11" s="13">
+        <v>6.8</v>
+      </c>
+      <c r="D11" s="13">
+        <v>16.3</v>
       </c>
       <c r="E11" s="4">
-        <v>0.0</v>
+        <v>9.4</v>
       </c>
       <c r="F11" s="4">
-        <v>0.0</v>
+        <v>4.4</v>
       </c>
       <c r="G11" s="4">
         <v>0.0</v>
@@ -3404,17 +3983,17 @@
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="11">
-        <v>8.9</v>
-      </c>
-      <c r="D12" s="11">
-        <v>24.2</v>
-      </c>
-      <c r="E12" s="11">
-        <v>96.4</v>
-      </c>
-      <c r="F12" s="11">
-        <v>93.1</v>
+      <c r="C12" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="D12" s="13">
+        <v>37.1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>83.7</v>
+      </c>
+      <c r="F12" s="13">
+        <v>87.9</v>
       </c>
       <c r="G12" s="4">
         <v>0.0</v>
@@ -3425,15 +4004,15 @@
         <v>46</v>
       </c>
       <c r="C13" s="4">
-        <v>0.0</v>
+        <v>2.2</v>
       </c>
       <c r="D13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="13">
         <v>3.6</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="13">
         <v>6.9</v>
       </c>
       <c r="G13" s="4">
@@ -3489,440 +4068,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-      <c r="G2">
-        <v>1.0</v>
+      <c r="B2" s="14">
+        <v>2.43</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2.43</v>
+      </c>
+      <c r="D2" s="14">
+        <v>3.71</v>
+      </c>
+      <c r="E2" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1.92</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.0</v>
       </c>
       <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3">
-        <v>1.67</v>
-      </c>
-      <c r="E3">
-        <v>1.67</v>
-      </c>
-      <c r="F3">
-        <v>1.67</v>
-      </c>
-      <c r="G3">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4">
-        <v>2.38</v>
-      </c>
-      <c r="E4">
-        <v>2.38</v>
-      </c>
-      <c r="F4">
-        <v>2.38</v>
-      </c>
-      <c r="G4">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D5">
-        <v>6.33</v>
-      </c>
-      <c r="E5">
-        <v>6.33</v>
-      </c>
-      <c r="F5">
-        <v>6.33</v>
-      </c>
-      <c r="G5">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D6">
-        <v>1.0</v>
-      </c>
-      <c r="E6">
-        <v>1.0</v>
-      </c>
-      <c r="F6">
-        <v>1.0</v>
-      </c>
-      <c r="G6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7">
-        <v>1.55</v>
-      </c>
-      <c r="E7">
-        <v>1.55</v>
-      </c>
-      <c r="F7">
-        <v>1.55</v>
-      </c>
-      <c r="G7">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D8">
-        <v>2.18</v>
-      </c>
-      <c r="E8">
-        <v>2.18</v>
-      </c>
-      <c r="F8">
-        <v>2.18</v>
-      </c>
-      <c r="G8">
-        <v>2.18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D9">
-        <v>6.39</v>
-      </c>
-      <c r="E9">
-        <v>6.39</v>
-      </c>
-      <c r="F9">
-        <v>6.39</v>
-      </c>
-      <c r="G9">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D10">
-        <v>1.0</v>
-      </c>
-      <c r="E10">
-        <v>1.0</v>
-      </c>
-      <c r="F10">
-        <v>1.0</v>
-      </c>
-      <c r="G10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D11">
-        <v>1.0</v>
-      </c>
-      <c r="E11">
-        <v>1.0</v>
-      </c>
-      <c r="F11">
-        <v>1.0</v>
-      </c>
-      <c r="G11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D12">
-        <v>2.79</v>
-      </c>
-      <c r="E12">
-        <v>2.79</v>
-      </c>
-      <c r="F12">
-        <v>2.79</v>
-      </c>
-      <c r="G12">
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D13">
-        <v>6.01</v>
-      </c>
-      <c r="E13">
-        <v>6.01</v>
-      </c>
-      <c r="F13">
-        <v>6.01</v>
-      </c>
-      <c r="G13">
-        <v>6.01</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D14">
-        <v>1.0</v>
-      </c>
-      <c r="E14">
-        <v>1.0</v>
-      </c>
-      <c r="F14">
-        <v>1.0</v>
-      </c>
-      <c r="G14">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D15">
-        <v>1.0</v>
-      </c>
-      <c r="E15">
-        <v>1.0</v>
-      </c>
-      <c r="F15">
-        <v>1.0</v>
-      </c>
-      <c r="G15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D16">
-        <v>1.0</v>
-      </c>
-      <c r="E16">
-        <v>1.0</v>
-      </c>
-      <c r="F16">
-        <v>1.0</v>
-      </c>
-      <c r="G16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D17">
-        <v>1.0</v>
-      </c>
-      <c r="E17">
-        <v>1.0</v>
-      </c>
-      <c r="F17">
-        <v>1.0</v>
-      </c>
-      <c r="G17">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D18">
-        <v>1.0</v>
-      </c>
-      <c r="E18">
-        <v>1.0</v>
-      </c>
-      <c r="F18">
-        <v>1.0</v>
-      </c>
-      <c r="G18">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D19">
-        <v>1.0</v>
-      </c>
-      <c r="E19">
-        <v>1.0</v>
-      </c>
-      <c r="F19">
-        <v>1.0</v>
-      </c>
-      <c r="G19">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D20">
-        <v>1.86</v>
-      </c>
-      <c r="E20">
-        <v>1.86</v>
-      </c>
-      <c r="F20">
-        <v>1.86</v>
-      </c>
-      <c r="G20">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D21">
-        <v>3.01</v>
-      </c>
-      <c r="E21">
-        <v>3.01</v>
-      </c>
-      <c r="F21">
-        <v>3.01</v>
-      </c>
-      <c r="G21">
-        <v>3.01</v>
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -3991,16 +4192,16 @@
         <v>1.0</v>
       </c>
       <c r="D3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="E3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="F3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="G3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="4">
@@ -4011,16 +4212,16 @@
         <v>1.0</v>
       </c>
       <c r="D4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="E4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="F4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="G4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="5">
@@ -4031,16 +4232,16 @@
         <v>1.0</v>
       </c>
       <c r="D5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="E5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="F5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="G5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="6">
@@ -4074,16 +4275,16 @@
         <v>1.0</v>
       </c>
       <c r="D7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="E7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="F7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="G7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="8">
@@ -4094,16 +4295,16 @@
         <v>1.0</v>
       </c>
       <c r="D8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="E8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="F8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="G8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="9">
@@ -4114,16 +4315,16 @@
         <v>1.0</v>
       </c>
       <c r="D9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="E9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="F9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="G9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
     </row>
     <row r="10">
@@ -4177,16 +4378,16 @@
         <v>1.0</v>
       </c>
       <c r="D12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="E12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="F12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="G12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="13">
@@ -4197,16 +4398,16 @@
         <v>1.0</v>
       </c>
       <c r="D13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="E13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="F13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="G13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="14">
@@ -4323,16 +4524,16 @@
         <v>1.0</v>
       </c>
       <c r="D19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="E19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="F19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="G19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
@@ -4343,16 +4544,16 @@
         <v>1.0</v>
       </c>
       <c r="D20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="E20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="F20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="G20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="21">
@@ -4363,16 +4564,16 @@
         <v>1.0</v>
       </c>
       <c r="D21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="E21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="F21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="G21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
     </row>
   </sheetData>
@@ -4386,9 +4587,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="2" width="24.29"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
@@ -4415,342 +4613,342 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="2">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D2">
+        <v>1.0</v>
+      </c>
+      <c r="E2">
+        <v>1.0</v>
+      </c>
+      <c r="F2">
+        <v>1.0</v>
+      </c>
+      <c r="G2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D3">
+        <v>1.6</v>
+      </c>
+      <c r="E3">
+        <v>1.6</v>
+      </c>
+      <c r="F3">
+        <v>1.6</v>
+      </c>
+      <c r="G3">
+        <v>1.6</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
-        <v>1.83</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D4">
+        <v>3.41</v>
+      </c>
+      <c r="E4">
+        <v>3.41</v>
+      </c>
+      <c r="F4">
+        <v>3.41</v>
+      </c>
+      <c r="G4">
+        <v>3.41</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
-        <v>10.88</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D5">
+        <v>12.33</v>
+      </c>
+      <c r="E5">
+        <v>12.33</v>
+      </c>
+      <c r="F5">
+        <v>12.33</v>
+      </c>
+      <c r="G5">
+        <v>12.33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G6" s="2">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D6">
+        <v>1.0</v>
+      </c>
+      <c r="E6">
+        <v>1.0</v>
+      </c>
+      <c r="F6">
+        <v>1.0</v>
+      </c>
+      <c r="G6">
         <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D7">
+        <v>1.92</v>
+      </c>
+      <c r="E7">
+        <v>1.92</v>
+      </c>
+      <c r="F7">
+        <v>1.92</v>
+      </c>
+      <c r="G7">
+        <v>1.92</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
-        <v>1.83</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D8">
+        <v>4.66</v>
+      </c>
+      <c r="E8">
+        <v>4.66</v>
+      </c>
+      <c r="F8">
+        <v>4.66</v>
+      </c>
+      <c r="G8">
+        <v>4.66</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
-        <v>10.88</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D9">
+        <v>9.68</v>
+      </c>
+      <c r="E9">
+        <v>9.68</v>
+      </c>
+      <c r="F9">
+        <v>9.68</v>
+      </c>
+      <c r="G9">
+        <v>9.68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="2">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D10">
+        <v>1.0</v>
+      </c>
+      <c r="E10">
+        <v>1.0</v>
+      </c>
+      <c r="F10">
+        <v>1.0</v>
+      </c>
+      <c r="G10">
         <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D11">
+        <v>1.0</v>
+      </c>
+      <c r="E11">
+        <v>1.0</v>
+      </c>
+      <c r="F11">
+        <v>1.0</v>
+      </c>
+      <c r="G11">
         <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
-        <v>1.83</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D12">
+        <v>2.58</v>
+      </c>
+      <c r="E12">
+        <v>2.58</v>
+      </c>
+      <c r="F12">
+        <v>2.58</v>
+      </c>
+      <c r="G12">
+        <v>2.58</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2">
-        <v>10.88</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D13">
+        <v>9.63</v>
+      </c>
+      <c r="E13">
+        <v>9.63</v>
+      </c>
+      <c r="F13">
+        <v>9.63</v>
+      </c>
+      <c r="G13">
+        <v>9.63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14">
-        <v>1.0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G14" s="2">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <v>1.0</v>
+      </c>
+      <c r="E14">
+        <v>1.0</v>
+      </c>
+      <c r="F14">
+        <v>1.0</v>
+      </c>
+      <c r="G14">
         <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D15">
+        <v>1.0</v>
+      </c>
+      <c r="E15">
+        <v>1.0</v>
+      </c>
+      <c r="F15">
+        <v>1.0</v>
+      </c>
+      <c r="G15">
         <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2">
-        <v>1.83</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G16" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D16">
+        <v>1.0</v>
+      </c>
+      <c r="E16">
+        <v>1.0</v>
+      </c>
+      <c r="F16">
+        <v>1.0</v>
+      </c>
+      <c r="G16">
         <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
-        <v>10.88</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D17">
+        <v>1.0</v>
+      </c>
+      <c r="E17">
+        <v>1.0</v>
+      </c>
+      <c r="F17">
+        <v>1.0</v>
+      </c>
+      <c r="G17">
         <v>1.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -4770,228 +4968,62 @@
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
       </c>
-      <c r="D19" s="2">
-        <v>1.26</v>
+      <c r="D19">
+        <v>1.65</v>
       </c>
       <c r="E19">
-        <v>1.0</v>
+        <v>1.65</v>
       </c>
       <c r="F19">
-        <v>1.0</v>
+        <v>1.65</v>
       </c>
       <c r="G19">
-        <v>1.0</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
       </c>
-      <c r="D20" s="2">
-        <v>1.83</v>
+      <c r="D20">
+        <v>2.73</v>
       </c>
       <c r="E20">
-        <v>1.0</v>
+        <v>2.73</v>
       </c>
       <c r="F20">
-        <v>1.0</v>
+        <v>2.73</v>
       </c>
       <c r="G20">
-        <v>1.0</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
       </c>
-      <c r="D21" s="2">
-        <v>10.88</v>
+      <c r="D21">
+        <v>11.21</v>
       </c>
       <c r="E21">
-        <v>2.1</v>
+        <v>11.21</v>
       </c>
       <c r="F21">
-        <v>2.1</v>
+        <v>11.21</v>
       </c>
       <c r="G21">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D22">
-        <v>1.0</v>
-      </c>
-      <c r="E22">
-        <v>1.0</v>
-      </c>
-      <c r="F22">
-        <v>1.0</v>
-      </c>
-      <c r="G22">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D23">
-        <v>1.66</v>
-      </c>
-      <c r="E23">
-        <v>1.0</v>
-      </c>
-      <c r="F23">
-        <v>1.0</v>
-      </c>
-      <c r="G23">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D24">
-        <v>2.5</v>
-      </c>
-      <c r="E24">
-        <v>1.0</v>
-      </c>
-      <c r="F24">
-        <v>1.0</v>
-      </c>
-      <c r="G24">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D25">
-        <v>14.97</v>
-      </c>
-      <c r="E25">
-        <v>1.92</v>
-      </c>
-      <c r="F25">
-        <v>1.92</v>
-      </c>
-      <c r="G25">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D26">
-        <v>1.0</v>
-      </c>
-      <c r="E26">
-        <v>1.0</v>
-      </c>
-      <c r="F26">
-        <v>1.0</v>
-      </c>
-      <c r="G26">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D27">
-        <v>1.0</v>
-      </c>
-      <c r="E27">
-        <v>1.0</v>
-      </c>
-      <c r="F27">
-        <v>1.0</v>
-      </c>
-      <c r="G27">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D28">
-        <v>1.0</v>
-      </c>
-      <c r="E28">
-        <v>1.0</v>
-      </c>
-      <c r="F28">
-        <v>1.0</v>
-      </c>
-      <c r="G28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D29">
-        <v>1.0</v>
-      </c>
-      <c r="E29">
-        <v>1.0</v>
-      </c>
-      <c r="F29">
-        <v>1.0</v>
-      </c>
-      <c r="G29">
-        <v>1.0</v>
+        <v>11.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>